<commit_message>
Save 03 10 2025
</commit_message>
<xml_diff>
--- a/4 четверть_10_GitLab.xlsx
+++ b/4 четверть_10_GitLab.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AlexServHW\Desktop\GB_Developer_Workbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E8AAD0F-F802-4A39-B5F0-77375CAB434E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E9B070A-6BA8-41A3-A2D2-A10A9DCB7C6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13050" yWindow="-19755" windowWidth="20745" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Название 1-3" sheetId="12" r:id="rId1"/>
@@ -20,12 +20,15 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="293">
   <si>
     <t>Урок 1 часть 1</t>
   </si>
@@ -2893,17 +2896,718 @@
     <t>При использовании локального GitLab и GitLab Runner’ов в случае появления
 проблем с GitLab Runner’ами можно включить debug-режим.</t>
   </si>
+  <si>
+    <t>Job</t>
+  </si>
+  <si>
+    <t>lesson6</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Пояснение!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Каждый job исполняется последовательно, либо параллельно друг другу</t>
+    </r>
+  </si>
+  <si>
+    <t>script:</t>
+  </si>
+  <si>
+    <t>before_script:</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">run_tests:
+  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>before_script: //код командной оболочки, который исполнится до основного скрипта</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+    - echo "Preparing test data"
+  script:
+    - echo "Running tests"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>run_tests: //название job</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+  script:
+    - echo "Running tests"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">run_tests:
+  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>script: //код командной оболочки</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+    - echo "Running tests"</t>
+    </r>
+  </si>
+  <si>
+    <t>Название job</t>
+  </si>
+  <si>
+    <t>Define commands that run after each job, including failed jobs</t>
+  </si>
+  <si>
+    <t>Commands that should run before script command</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+</t>
+  </si>
+  <si>
+    <t>Pipeline</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Pipeline</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> contains </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>jobs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">.
+You can define as many </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>jobs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> as you want.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">run_tests:
+  before_script:
+    - echo "Preparing test data"
+  script:
+    - echo "Running tests"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  after_script:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+    - echo "Cleaning up temporary files"</t>
+    </r>
+  </si>
+  <si>
+    <t>after_script:</t>
+  </si>
+  <si>
+    <t>run_tests:
+  before_script:
+    - echo "Preparing test data"
+  script:
+    - echo "Running tests"
+  after_script:
+    - echo "Cleaning up temporary files"
+build_image:
+  script:
+    - echo "Running the docker image..."
+    - echo "Tagging the docker image"
+push-image:
+  script:
+    - echo "Logging into docker registry"
+    - echo "Pushing docker image to registry"</t>
+  </si>
+  <si>
+    <t>lesson7</t>
+  </si>
+  <si>
+    <t>Gitlab runner
+-Установка
+-Регистрация</t>
+  </si>
+  <si>
+    <t>Установка</t>
+  </si>
+  <si>
+    <t>Регистрация</t>
+  </si>
+  <si>
+    <t>curl -LJO "https://s3.dualstack.us-east-1.amazonaws.com/gitlab-runner-downloads/latest/deb/gitlab-runner-helper-images.deb"
+curl -LJO "https://s3.dualstack.us-east-1.amazonaws.com/gitlab-runner-downloads/latest/deb/gitlab-runner_${arch}.deb"</t>
+  </si>
+  <si>
+    <t>Скачиваем dpkg архивы</t>
+  </si>
+  <si>
+    <t>Ручная установка</t>
+  </si>
+  <si>
+    <t>`https://docs.gitlab.com/runner/install/linux-manually/</t>
+  </si>
+  <si>
+    <t>dpkg -i gitlab-runner-helper-images.deb gitlab-runner_&lt;arch&gt;.deb</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Шаг 2
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Подсказка!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Команда, чтобы узнать архитектуру процессора
+dpkg --print-architecture</t>
+    </r>
+  </si>
+  <si>
+    <t>`https://docs.gitlab.com/runner/install/linux-repository/</t>
+  </si>
+  <si>
+    <t>Обычная установка</t>
+  </si>
+  <si>
+    <t>curl -L "https://packages.gitlab.com/install/repositories/runner/gitlab-runner/script.deb.sh" | sudo bash</t>
+  </si>
+  <si>
+    <t>sudo apt install gitlab-runner</t>
+  </si>
+  <si>
+    <r>
+      <t>Установка gitlub-runner
+dpkg -i gitlab-runner-helper-images.deb gitlab-runner_</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>amd64</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.deb</t>
+    </r>
+  </si>
+  <si>
+    <t>Установка gitlub-runner</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Подсказка!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> gitlab-runner располагается в /etc/gitlab-runner/config.toml</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Подсказка!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> sudo gitlab-runner status - узнать статус работы gitlab runner</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Регистрируем новый gitlab-runner
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Указываем конкретные тэги, которые будут установлены в jobs
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Указываем не использовать конкретные тэги - брать в работу все jobs
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Выбираем ОС сервера, где установлен gitlab-runner
+</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Любые jobs (даже без тэгов)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> будут обработаны gitlab runner
+run_tests:
+  before_script:
+    - echo "Preparing test data"
+  script:
+    - echo "Running tests"
+  after_script:
+    - echo "Cleaning up temporary files"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Только jobs с тэгом test</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> будут обработаны gitlab runner
+run_tests:
+  before_script:
+    - echo "Preparing test data"
+  script:
+    - echo "Running tests"
+  after_script:
+    - echo "Cleaning up temporary files"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  tags:
+    - test</t>
+    </r>
+  </si>
+  <si>
+    <t>(в gitlab проекте)</t>
+  </si>
+  <si>
+    <t>(на сервере)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">gitlab-runner register </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> --url https://gitlab.hwcompany.ru</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>--token</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> glrt-t3_cZ4RxBynwr_8ADa6KR7G</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Шаг 4
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Пояснение!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Устаналиваем в /etc/gitlab-runner/config.toml настройки нашего зарегистрированного проекте gitlab-runner, используя полученный в gitlab </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>токен</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> и </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>url</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Шаг 2 Вариант 2
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Очень важно!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Или не ограничивать</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Шаг 2 Вариант 1 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Очень важно!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Ограничивать по конкретным тэгам...</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -3057,8 +3761,26 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3101,6 +3823,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -3113,9 +3841,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -3126,44 +3854,44 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
@@ -3172,11 +3900,20 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -3184,26 +3921,32 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3268,13 +4011,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>97157</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>81</xdr:row>
       <xdr:rowOff>50568</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>3181350</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>81</xdr:row>
       <xdr:rowOff>705621</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3312,13 +4055,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>150495</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>88</xdr:row>
       <xdr:rowOff>127019</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>2187301</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>88</xdr:row>
       <xdr:rowOff>1449939</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3356,13 +4099,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>2403240</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>88</xdr:row>
       <xdr:rowOff>87630</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>4397222</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>88</xdr:row>
       <xdr:rowOff>1389067</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3400,13 +4143,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>97155</xdr:colOff>
-      <xdr:row>73</xdr:row>
+      <xdr:row>119</xdr:row>
       <xdr:rowOff>106571</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>2800350</xdr:colOff>
-      <xdr:row>73</xdr:row>
+      <xdr:row>119</xdr:row>
       <xdr:rowOff>1882242</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3444,13 +4187,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>73</xdr:row>
+      <xdr:row>119</xdr:row>
       <xdr:rowOff>556076</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>3751173</xdr:colOff>
-      <xdr:row>73</xdr:row>
+      <xdr:row>119</xdr:row>
       <xdr:rowOff>1234440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3488,13 +4231,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>324154</xdr:colOff>
-      <xdr:row>79</xdr:row>
+      <xdr:row>125</xdr:row>
       <xdr:rowOff>62865</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>3449396</xdr:colOff>
-      <xdr:row>79</xdr:row>
+      <xdr:row>125</xdr:row>
       <xdr:rowOff>2476500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3532,13 +4275,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>940331</xdr:colOff>
-      <xdr:row>79</xdr:row>
+      <xdr:row>125</xdr:row>
       <xdr:rowOff>219075</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>2856052</xdr:colOff>
-      <xdr:row>79</xdr:row>
+      <xdr:row>125</xdr:row>
       <xdr:rowOff>1047945</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3576,13 +4319,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>948689</xdr:colOff>
-      <xdr:row>79</xdr:row>
+      <xdr:row>125</xdr:row>
       <xdr:rowOff>1346743</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>2004059</xdr:colOff>
-      <xdr:row>79</xdr:row>
+      <xdr:row>125</xdr:row>
       <xdr:rowOff>2514732</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3620,13 +4363,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>207645</xdr:colOff>
-      <xdr:row>118</xdr:row>
+      <xdr:row>164</xdr:row>
       <xdr:rowOff>1355890</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>4743207</xdr:colOff>
-      <xdr:row>118</xdr:row>
+      <xdr:row>164</xdr:row>
       <xdr:rowOff>2724150</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3664,13 +4407,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>127</xdr:row>
+      <xdr:row>173</xdr:row>
       <xdr:rowOff>72390</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>2918147</xdr:colOff>
-      <xdr:row>127</xdr:row>
+      <xdr:row>173</xdr:row>
       <xdr:rowOff>662940</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3708,13 +4451,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>139332</xdr:colOff>
-      <xdr:row>132</xdr:row>
+      <xdr:row>178</xdr:row>
       <xdr:rowOff>139961</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>3392670</xdr:colOff>
-      <xdr:row>132</xdr:row>
+      <xdr:row>178</xdr:row>
       <xdr:rowOff>1314898</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3752,13 +4495,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>119453</xdr:colOff>
-      <xdr:row>140</xdr:row>
+      <xdr:row>186</xdr:row>
       <xdr:rowOff>77293</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>2644566</xdr:colOff>
-      <xdr:row>140</xdr:row>
+      <xdr:row>186</xdr:row>
       <xdr:rowOff>1430322</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3796,13 +4539,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>93232</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>73</xdr:row>
       <xdr:rowOff>95362</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>3122942</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>73</xdr:row>
       <xdr:rowOff>1201159</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3840,13 +4583,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1014288</xdr:colOff>
-      <xdr:row>152</xdr:row>
+      <xdr:row>198</xdr:row>
       <xdr:rowOff>56938</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>2764522</xdr:colOff>
-      <xdr:row>152</xdr:row>
+      <xdr:row>198</xdr:row>
       <xdr:rowOff>701311</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3884,13 +4627,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>128712</xdr:colOff>
-      <xdr:row>152</xdr:row>
+      <xdr:row>198</xdr:row>
       <xdr:rowOff>49764</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1311167</xdr:colOff>
-      <xdr:row>152</xdr:row>
+      <xdr:row>198</xdr:row>
       <xdr:rowOff>669349</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3928,13 +4671,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>145277</xdr:colOff>
-      <xdr:row>155</xdr:row>
+      <xdr:row>201</xdr:row>
       <xdr:rowOff>71919</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1560940</xdr:colOff>
-      <xdr:row>155</xdr:row>
+      <xdr:row>201</xdr:row>
       <xdr:rowOff>970926</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3972,13 +4715,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>340249</xdr:colOff>
-      <xdr:row>165</xdr:row>
+      <xdr:row>211</xdr:row>
       <xdr:rowOff>219159</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>2705642</xdr:colOff>
-      <xdr:row>165</xdr:row>
+      <xdr:row>211</xdr:row>
       <xdr:rowOff>1009817</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4016,13 +4759,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>159275</xdr:colOff>
-      <xdr:row>168</xdr:row>
+      <xdr:row>214</xdr:row>
       <xdr:rowOff>248479</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>3373289</xdr:colOff>
-      <xdr:row>168</xdr:row>
+      <xdr:row>214</xdr:row>
       <xdr:rowOff>608554</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4060,13 +4803,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>149086</xdr:colOff>
-      <xdr:row>168</xdr:row>
+      <xdr:row>214</xdr:row>
       <xdr:rowOff>578733</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>2955043</xdr:colOff>
-      <xdr:row>168</xdr:row>
+      <xdr:row>214</xdr:row>
       <xdr:rowOff>1201643</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4104,13 +4847,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>41413</xdr:colOff>
-      <xdr:row>171</xdr:row>
+      <xdr:row>217</xdr:row>
       <xdr:rowOff>132522</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>3295435</xdr:colOff>
-      <xdr:row>171</xdr:row>
+      <xdr:row>217</xdr:row>
       <xdr:rowOff>494503</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4148,13 +4891,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>64355</xdr:colOff>
-      <xdr:row>173</xdr:row>
+      <xdr:row>219</xdr:row>
       <xdr:rowOff>84732</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>3372370</xdr:colOff>
-      <xdr:row>173</xdr:row>
+      <xdr:row>219</xdr:row>
       <xdr:rowOff>510954</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4192,13 +4935,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>132521</xdr:colOff>
-      <xdr:row>174</xdr:row>
+      <xdr:row>220</xdr:row>
       <xdr:rowOff>35036</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>2209151</xdr:colOff>
-      <xdr:row>174</xdr:row>
+      <xdr:row>220</xdr:row>
       <xdr:rowOff>608492</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4236,13 +4979,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>208969</xdr:colOff>
-      <xdr:row>164</xdr:row>
+      <xdr:row>210</xdr:row>
       <xdr:rowOff>207728</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>4859836</xdr:colOff>
-      <xdr:row>164</xdr:row>
+      <xdr:row>210</xdr:row>
       <xdr:rowOff>1276184</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4268,6 +5011,221 @@
         <a:xfrm>
           <a:off x="6147599" y="111617098"/>
           <a:ext cx="4643247" cy="1076076"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>25063</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3182794" cy="704851"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="27" name="Picture 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD3E5545-2DF7-4D2B-B7E5-15C3731246B9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5959138" y="9496424"/>
+          <a:ext cx="3182794" cy="704851"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>121920</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>258601</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1304036</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>1044615</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="28" name="Picture 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E868192A-815B-45D1-970A-8A3A6C1DAFFE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6057900" y="22569961"/>
+          <a:ext cx="1182116" cy="786014"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>82803</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3192976</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>1661160</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="29" name="Picture 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D12D1FB2-6085-4A32-8806-07EE1D040EED}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6018783" y="23599140"/>
+          <a:ext cx="3110173" cy="1470660"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>95122</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>205740</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2543624</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>1409700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="32" name="Picture 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4D9314F-8B6E-4D99-BCC1-57C5E81005FB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6031102" y="25443180"/>
+          <a:ext cx="2448502" cy="1203960"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>137160</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>259458</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1273396</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>1021653</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="33" name="Picture 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3E6B523-7475-4BCA-9B0E-4E5E6AE5EE8A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6073140" y="25862658"/>
+          <a:ext cx="1136236" cy="762195"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4545,10 +5503,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:V175"/>
+  <dimension ref="A2:V221"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A153" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B162" sqref="B162"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
@@ -4714,7 +5672,7 @@
       </c>
       <c r="C16" s="9"/>
     </row>
-    <row r="17" spans="1:21">
+    <row r="17" spans="1:22">
       <c r="B17" s="2" t="s">
         <v>9</v>
       </c>
@@ -4722,7 +5680,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:21">
+    <row r="19" spans="1:22">
       <c r="A19" s="3"/>
       <c r="B19" s="5"/>
       <c r="C19" s="6"/>
@@ -4741,1179 +5699,1496 @@
       <c r="S19" s="5"/>
       <c r="U19" s="5"/>
     </row>
-    <row r="20" spans="1:21">
-      <c r="C20" s="22" t="s">
+    <row r="20" spans="1:22">
+      <c r="C20" s="31" t="s">
+        <v>247</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="P20" s="1"/>
+      <c r="U20" s="1"/>
+      <c r="V20" s="2"/>
+    </row>
+    <row r="21" spans="1:22">
+      <c r="A21" s="18" t="s">
+        <v>259</v>
+      </c>
+      <c r="C21" s="2"/>
+      <c r="P21" s="1"/>
+      <c r="U21" s="1"/>
+      <c r="V21" s="2"/>
+    </row>
+    <row r="22" spans="1:22" ht="57.6">
+      <c r="A22" s="2"/>
+      <c r="B22" s="30" t="s">
+        <v>260</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="P22" s="1"/>
+      <c r="U22" s="1"/>
+      <c r="V22" s="2"/>
+    </row>
+    <row r="23" spans="1:22">
+      <c r="A23" s="18" t="s">
+        <v>247</v>
+      </c>
+      <c r="C23" s="2"/>
+      <c r="P23" s="1"/>
+      <c r="U23" s="1"/>
+      <c r="V23" s="2"/>
+    </row>
+    <row r="24" spans="1:22" ht="43.2">
+      <c r="A24" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="C24" s="30" t="s">
+        <v>253</v>
+      </c>
+      <c r="P24" s="1"/>
+      <c r="U24" s="1"/>
+      <c r="V24" s="2"/>
+    </row>
+    <row r="25" spans="1:22" ht="43.2">
+      <c r="A25" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="C25" s="30" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" ht="86.4">
+      <c r="A26" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="C26" s="30" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" ht="100.8">
+      <c r="A27" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="C27" s="30" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22">
+      <c r="A28" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28" s="30"/>
+    </row>
+    <row r="29" spans="1:22" ht="244.8">
+      <c r="B29" s="30" t="s">
+        <v>249</v>
+      </c>
+      <c r="C29" s="30" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22">
+      <c r="A30" s="3"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="3"/>
+      <c r="N30" s="3"/>
+      <c r="P30" s="5"/>
+      <c r="Q30" s="5"/>
+      <c r="R30" s="5"/>
+      <c r="S30" s="5"/>
+      <c r="U30" s="5"/>
+    </row>
+    <row r="31" spans="1:22" ht="43.2">
+      <c r="C31" s="31" t="s">
+        <v>265</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="P31" s="1"/>
+      <c r="U31" s="1"/>
+      <c r="V31" s="2"/>
+    </row>
+    <row r="32" spans="1:22">
+      <c r="A32" s="18" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21">
+      <c r="A33" s="32" t="s">
+        <v>275</v>
+      </c>
+      <c r="C33" s="1"/>
+      <c r="D33" s="30" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" ht="57.6">
+      <c r="A34" s="30" t="s">
+        <v>276</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C34" s="30" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21">
+      <c r="A35" s="30" t="s">
+        <v>277</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" s="30" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21">
+      <c r="A36" s="32" t="s">
+        <v>270</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" ht="115.2">
+      <c r="A37" s="30" t="s">
+        <v>268</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C37" s="30" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" ht="57.6">
+      <c r="A38" s="30" t="s">
+        <v>272</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="C38" s="30" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21">
+      <c r="A39" s="18" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" ht="28.8">
+      <c r="C40" s="30" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" ht="86.4">
+      <c r="A41" s="33" t="s">
+        <v>287</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C41" s="30" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" ht="144">
+      <c r="A42" s="33" t="s">
+        <v>287</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="C42" s="30" t="s">
+        <v>282</v>
+      </c>
+      <c r="D42" s="30" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" ht="115.2">
+      <c r="A43" s="33" t="s">
+        <v>287</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="C43" s="30" t="s">
+        <v>283</v>
+      </c>
+      <c r="D43" s="30" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" ht="86.4">
+      <c r="A44" s="33" t="s">
+        <v>287</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C44" s="30" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" ht="72">
+      <c r="A45" s="34" t="s">
+        <v>288</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="C45" s="30" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" ht="28.8">
+      <c r="C46" s="30" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21">
+      <c r="A48" s="3"/>
+      <c r="B48" s="5"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="3"/>
+      <c r="F48" s="3"/>
+      <c r="G48" s="5"/>
+      <c r="H48" s="3"/>
+      <c r="I48" s="3"/>
+      <c r="K48" s="3"/>
+      <c r="L48" s="3"/>
+      <c r="M48" s="3"/>
+      <c r="N48" s="3"/>
+      <c r="P48" s="5"/>
+      <c r="Q48" s="5"/>
+      <c r="R48" s="5"/>
+      <c r="S48" s="5"/>
+      <c r="U48" s="5"/>
+    </row>
+    <row r="49" spans="3:22" ht="43.2">
+      <c r="C49" s="31" t="s">
+        <v>265</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="P49" s="1"/>
+      <c r="U49" s="1"/>
+      <c r="V49" s="2"/>
+    </row>
+    <row r="65" spans="1:22">
+      <c r="A65" s="3"/>
+      <c r="B65" s="5"/>
+      <c r="C65" s="6"/>
+      <c r="D65" s="3"/>
+      <c r="F65" s="3"/>
+      <c r="G65" s="5"/>
+      <c r="H65" s="3"/>
+      <c r="I65" s="3"/>
+      <c r="K65" s="3"/>
+      <c r="L65" s="3"/>
+      <c r="M65" s="3"/>
+      <c r="N65" s="3"/>
+      <c r="P65" s="5"/>
+      <c r="Q65" s="5"/>
+      <c r="R65" s="5"/>
+      <c r="S65" s="5"/>
+      <c r="U65" s="5"/>
+    </row>
+    <row r="66" spans="1:22">
+      <c r="C66" s="22" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="21" spans="1:21">
-      <c r="C21" s="23" t="s">
+    <row r="67" spans="1:22">
+      <c r="C67" s="23" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="22" spans="1:21">
-      <c r="C22" s="23" t="s">
+    <row r="68" spans="1:22">
+      <c r="C68" s="23" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="57.6">
-      <c r="C23" s="23" t="s">
+    <row r="69" spans="1:22" ht="57.6">
+      <c r="C69" s="23" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="24" spans="1:21" ht="28.8">
-      <c r="C24" s="23" t="s">
+    <row r="70" spans="1:22" ht="28.8">
+      <c r="C70" s="23" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="25" spans="1:21" ht="28.8">
-      <c r="B25" s="1"/>
-      <c r="C25" s="23" t="s">
+    <row r="71" spans="1:22" ht="28.8">
+      <c r="B71" s="1"/>
+      <c r="C71" s="23" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="26" spans="1:21" ht="158.4">
-      <c r="B26" s="2" t="s">
+    <row r="72" spans="1:22" ht="158.4">
+      <c r="B72" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="C26" s="23" t="s">
+      <c r="C72" s="23" t="s">
         <v>189</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D72" s="2" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="27" spans="1:21" ht="57.6">
-      <c r="C27" s="23" t="s">
+    <row r="73" spans="1:22" ht="57.6">
+      <c r="C73" s="23" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="28" spans="1:21" ht="100.8">
-      <c r="B28" s="2" t="s">
+    <row r="74" spans="1:22" ht="100.8">
+      <c r="B74" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="C28" s="23" t="s">
+      <c r="C74" s="23" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="32" spans="1:21">
-      <c r="A32" s="3"/>
-      <c r="B32" s="5"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="3"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="5"/>
-      <c r="H32" s="3"/>
-      <c r="I32" s="3"/>
-      <c r="K32" s="3"/>
-      <c r="L32" s="3"/>
-      <c r="M32" s="3"/>
-      <c r="N32" s="3"/>
-      <c r="P32" s="5"/>
-      <c r="Q32" s="5"/>
-      <c r="R32" s="5"/>
-      <c r="S32" s="5"/>
-      <c r="U32" s="5"/>
-    </row>
-    <row r="33" spans="1:22">
-      <c r="A33" s="1" t="s">
+    <row r="78" spans="1:22">
+      <c r="A78" s="3"/>
+      <c r="B78" s="5"/>
+      <c r="C78" s="6"/>
+      <c r="D78" s="3"/>
+      <c r="F78" s="3"/>
+      <c r="G78" s="5"/>
+      <c r="H78" s="3"/>
+      <c r="I78" s="3"/>
+      <c r="K78" s="3"/>
+      <c r="L78" s="3"/>
+      <c r="M78" s="3"/>
+      <c r="N78" s="3"/>
+      <c r="P78" s="5"/>
+      <c r="Q78" s="5"/>
+      <c r="R78" s="5"/>
+      <c r="S78" s="5"/>
+      <c r="U78" s="5"/>
+    </row>
+    <row r="79" spans="1:22">
+      <c r="A79" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C33" s="13" t="s">
+      <c r="C79" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="P33" s="1"/>
-      <c r="U33" s="1"/>
-      <c r="V33" s="2"/>
-    </row>
-    <row r="34" spans="1:22" ht="57.6">
-      <c r="C34" s="9" t="s">
+      <c r="P79" s="1"/>
+      <c r="U79" s="1"/>
+      <c r="V79" s="2"/>
+    </row>
+    <row r="80" spans="1:22" ht="57.6">
+      <c r="C80" s="9" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="1:22" ht="28.8">
-      <c r="C35" s="9" t="s">
+    <row r="81" spans="1:22" ht="28.8">
+      <c r="C81" s="9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:22" ht="57.6">
-      <c r="C36" s="9" t="s">
+    <row r="82" spans="1:22" ht="57.6">
+      <c r="C82" s="9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:22" ht="360">
-      <c r="C37" s="9" t="s">
+    <row r="83" spans="1:22" ht="360">
+      <c r="C83" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="D83" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:22">
-      <c r="C38" s="9"/>
-    </row>
-    <row r="39" spans="1:22">
-      <c r="A39" s="3"/>
-      <c r="B39" s="5"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="3"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="5"/>
-      <c r="H39" s="3"/>
-      <c r="I39" s="3"/>
-      <c r="K39" s="3"/>
-      <c r="L39" s="3"/>
-      <c r="M39" s="3"/>
-      <c r="N39" s="3"/>
-      <c r="P39" s="5"/>
-      <c r="Q39" s="5"/>
-      <c r="R39" s="5"/>
-      <c r="S39" s="5"/>
-      <c r="U39" s="5"/>
-    </row>
-    <row r="40" spans="1:22">
-      <c r="A40" s="1" t="s">
+    <row r="84" spans="1:22">
+      <c r="C84" s="9"/>
+    </row>
+    <row r="85" spans="1:22">
+      <c r="A85" s="3"/>
+      <c r="B85" s="5"/>
+      <c r="C85" s="6"/>
+      <c r="D85" s="3"/>
+      <c r="F85" s="3"/>
+      <c r="G85" s="5"/>
+      <c r="H85" s="3"/>
+      <c r="I85" s="3"/>
+      <c r="K85" s="3"/>
+      <c r="L85" s="3"/>
+      <c r="M85" s="3"/>
+      <c r="N85" s="3"/>
+      <c r="P85" s="5"/>
+      <c r="Q85" s="5"/>
+      <c r="R85" s="5"/>
+      <c r="S85" s="5"/>
+      <c r="U85" s="5"/>
+    </row>
+    <row r="86" spans="1:22">
+      <c r="A86" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C40" s="13" t="s">
+      <c r="C86" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="P40" s="1"/>
-      <c r="U40" s="1"/>
-      <c r="V40" s="2"/>
-    </row>
-    <row r="41" spans="1:22">
-      <c r="C41" s="9" t="s">
+      <c r="P86" s="1"/>
+      <c r="U86" s="1"/>
+      <c r="V86" s="2"/>
+    </row>
+    <row r="87" spans="1:22">
+      <c r="C87" s="9" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="42" spans="1:22" ht="288">
-      <c r="B42" s="2" t="s">
+    <row r="88" spans="1:22" ht="288">
+      <c r="B88" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C42" s="9" t="s">
+      <c r="C88" s="9" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="43" spans="1:22" ht="129.6">
-      <c r="B43" s="2" t="s">
+    <row r="89" spans="1:22" ht="129.6">
+      <c r="B89" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C43" s="9"/>
-    </row>
-    <row r="44" spans="1:22">
-      <c r="C44" s="9"/>
-    </row>
-    <row r="45" spans="1:22">
-      <c r="A45" s="3"/>
-      <c r="B45" s="5"/>
-      <c r="C45" s="6"/>
-      <c r="D45" s="3"/>
-      <c r="F45" s="3"/>
-      <c r="G45" s="5"/>
-      <c r="H45" s="3"/>
-      <c r="I45" s="3"/>
-      <c r="K45" s="3"/>
-      <c r="L45" s="3"/>
-      <c r="M45" s="3"/>
-      <c r="N45" s="3"/>
-      <c r="P45" s="5"/>
-      <c r="Q45" s="5"/>
-      <c r="R45" s="5"/>
-      <c r="S45" s="5"/>
-      <c r="U45" s="5"/>
-    </row>
-    <row r="46" spans="1:22">
-      <c r="A46" s="1" t="s">
+      <c r="C89" s="9"/>
+    </row>
+    <row r="90" spans="1:22">
+      <c r="C90" s="9"/>
+    </row>
+    <row r="91" spans="1:22">
+      <c r="A91" s="3"/>
+      <c r="B91" s="5"/>
+      <c r="C91" s="6"/>
+      <c r="D91" s="3"/>
+      <c r="F91" s="3"/>
+      <c r="G91" s="5"/>
+      <c r="H91" s="3"/>
+      <c r="I91" s="3"/>
+      <c r="K91" s="3"/>
+      <c r="L91" s="3"/>
+      <c r="M91" s="3"/>
+      <c r="N91" s="3"/>
+      <c r="P91" s="5"/>
+      <c r="Q91" s="5"/>
+      <c r="R91" s="5"/>
+      <c r="S91" s="5"/>
+      <c r="U91" s="5"/>
+    </row>
+    <row r="92" spans="1:22">
+      <c r="A92" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C46" s="17" t="s">
+      <c r="C92" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="P46" s="1"/>
-      <c r="U46" s="1"/>
-      <c r="V46" s="2"/>
-    </row>
-    <row r="47" spans="1:22">
-      <c r="A47" s="13" t="s">
+      <c r="P92" s="1"/>
+      <c r="U92" s="1"/>
+      <c r="V92" s="2"/>
+    </row>
+    <row r="93" spans="1:22">
+      <c r="A93" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C47" s="9"/>
-    </row>
-    <row r="48" spans="1:22" ht="72">
-      <c r="B48" s="9" t="s">
+      <c r="C93" s="9"/>
+    </row>
+    <row r="94" spans="1:22" ht="72">
+      <c r="B94" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="C48" s="9" t="s">
+      <c r="C94" s="9" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="28.8">
-      <c r="C49" s="9" t="s">
+    <row r="95" spans="1:22" ht="28.8">
+      <c r="C95" s="9" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="15">
-      <c r="A50" s="11" t="s">
+    <row r="96" spans="1:22" ht="15">
+      <c r="A96" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="B50" s="14" t="s">
+      <c r="B96" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="C50" s="14" t="s">
+      <c r="C96" s="14" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="15">
-      <c r="B51" s="15" t="s">
+    <row r="97" spans="1:3" ht="15">
+      <c r="B97" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C51" s="16" t="s">
+      <c r="C97" s="16" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="15">
-      <c r="B52" s="15" t="s">
+    <row r="98" spans="1:3" ht="15">
+      <c r="B98" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="C52" s="16" t="s">
+      <c r="C98" s="16" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="15">
-      <c r="B53" s="15" t="s">
+    <row r="99" spans="1:3" ht="15">
+      <c r="B99" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="C53" s="16" t="s">
+      <c r="C99" s="16" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="15">
-      <c r="B54" s="15" t="s">
+    <row r="100" spans="1:3" ht="15">
+      <c r="B100" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="C54" s="16" t="s">
+      <c r="C100" s="16" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="72">
-      <c r="A55" s="1" t="s">
+    <row r="101" spans="1:3" ht="72">
+      <c r="A101" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C55" s="9" t="s">
+      <c r="C101" s="9" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="15">
-      <c r="A56" s="11" t="s">
+    <row r="102" spans="1:3" ht="15">
+      <c r="A102" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="B56" s="14" t="s">
+      <c r="B102" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="C56" s="14" t="s">
+      <c r="C102" s="14" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="15">
-      <c r="B57" s="15" t="s">
+    <row r="103" spans="1:3" ht="15">
+      <c r="B103" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="C57" s="16" t="s">
+      <c r="C103" s="16" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="15">
-      <c r="B58" s="15" t="s">
+    <row r="104" spans="1:3" ht="15">
+      <c r="B104" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="C58" s="16" t="s">
+      <c r="C104" s="16" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="15">
-      <c r="B59" s="15" t="s">
+    <row r="105" spans="1:3" ht="15">
+      <c r="B105" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="C59" s="16" t="s">
+      <c r="C105" s="16" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="72">
-      <c r="A60" s="1" t="s">
+    <row r="106" spans="1:3" ht="72">
+      <c r="A106" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C60" s="9" t="s">
+      <c r="C106" s="9" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
-      <c r="A61" s="11" t="s">
+    <row r="107" spans="1:3">
+      <c r="A107" s="11" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
-      <c r="C62" s="9" t="s">
+    <row r="108" spans="1:3">
+      <c r="C108" s="9" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="15">
-      <c r="B63" s="14" t="s">
+    <row r="109" spans="1:3" ht="15">
+      <c r="B109" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="C63" s="14" t="s">
+      <c r="C109" s="14" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="15">
-      <c r="B64" s="15" t="s">
+    <row r="110" spans="1:3" ht="15">
+      <c r="B110" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="C64" s="16" t="s">
+      <c r="C110" s="16" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="65" spans="1:21" ht="15">
-      <c r="B65" s="15" t="s">
+    <row r="111" spans="1:3" ht="15">
+      <c r="B111" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="C65" s="16" t="s">
+      <c r="C111" s="16" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="66" spans="1:21">
-      <c r="A66" s="1" t="s">
+    <row r="112" spans="1:3">
+      <c r="A112" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="67" spans="1:21" ht="216">
-      <c r="B67" s="2" t="s">
+    <row r="113" spans="1:21" ht="216">
+      <c r="B113" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C67" s="9" t="s">
+      <c r="C113" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="D67" s="2" t="s">
+      <c r="D113" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="68" spans="1:21">
-      <c r="C68" s="9"/>
-      <c r="D68" s="2"/>
-    </row>
-    <row r="69" spans="1:21">
-      <c r="A69" s="3"/>
-      <c r="B69" s="5"/>
-      <c r="C69" s="6"/>
-      <c r="D69" s="3"/>
-      <c r="F69" s="3"/>
-      <c r="G69" s="5"/>
-      <c r="H69" s="3"/>
-      <c r="I69" s="3"/>
-      <c r="K69" s="3"/>
-      <c r="L69" s="3"/>
-      <c r="M69" s="3"/>
-      <c r="N69" s="3"/>
-      <c r="P69" s="5"/>
-      <c r="Q69" s="5"/>
-      <c r="R69" s="5"/>
-      <c r="S69" s="5"/>
-      <c r="U69" s="5"/>
-    </row>
-    <row r="70" spans="1:21">
-      <c r="A70" s="1" t="s">
+    <row r="114" spans="1:21">
+      <c r="C114" s="9"/>
+      <c r="D114" s="2"/>
+    </row>
+    <row r="115" spans="1:21">
+      <c r="A115" s="3"/>
+      <c r="B115" s="5"/>
+      <c r="C115" s="6"/>
+      <c r="D115" s="3"/>
+      <c r="F115" s="3"/>
+      <c r="G115" s="5"/>
+      <c r="H115" s="3"/>
+      <c r="I115" s="3"/>
+      <c r="K115" s="3"/>
+      <c r="L115" s="3"/>
+      <c r="M115" s="3"/>
+      <c r="N115" s="3"/>
+      <c r="P115" s="5"/>
+      <c r="Q115" s="5"/>
+      <c r="R115" s="5"/>
+      <c r="S115" s="5"/>
+      <c r="U115" s="5"/>
+    </row>
+    <row r="116" spans="1:21">
+      <c r="A116" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C70" s="17" t="s">
+      <c r="C116" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="D70" s="2"/>
-    </row>
-    <row r="71" spans="1:21">
-      <c r="A71" s="18" t="s">
+      <c r="D116" s="2"/>
+    </row>
+    <row r="117" spans="1:21">
+      <c r="A117" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="C71" s="9"/>
-      <c r="D71" s="2"/>
-    </row>
-    <row r="72" spans="1:21" ht="43.2">
-      <c r="A72" s="2"/>
-      <c r="B72" s="9" t="s">
+      <c r="C117" s="9"/>
+      <c r="D117" s="2"/>
+    </row>
+    <row r="118" spans="1:21" ht="43.2">
+      <c r="A118" s="2"/>
+      <c r="B118" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="C72" s="9" t="s">
+      <c r="C118" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="D72" s="2"/>
-    </row>
-    <row r="73" spans="1:21" ht="28.8">
-      <c r="A73" s="19" t="s">
+      <c r="D118" s="2"/>
+    </row>
+    <row r="119" spans="1:21" ht="28.8">
+      <c r="A119" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="C73" s="9"/>
-      <c r="D73" s="2"/>
-    </row>
-    <row r="74" spans="1:21" ht="158.4">
-      <c r="B74" s="2" t="s">
+      <c r="C119" s="9"/>
+      <c r="D119" s="2"/>
+    </row>
+    <row r="120" spans="1:21" ht="158.4">
+      <c r="B120" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D74" s="9" t="s">
+      <c r="D120" s="9" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="75" spans="1:21" ht="28.8">
-      <c r="A75" s="1" t="s">
+    <row r="121" spans="1:21" ht="28.8">
+      <c r="A121" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C75" s="9" t="s">
+      <c r="C121" s="9" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="76" spans="1:21" ht="28.8">
-      <c r="C76" s="9" t="s">
+    <row r="122" spans="1:21" ht="28.8">
+      <c r="C122" s="9" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="77" spans="1:21">
-      <c r="A77" s="1" t="s">
+    <row r="123" spans="1:21">
+      <c r="A123" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C77" s="9" t="s">
+      <c r="C123" s="9" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="78" spans="1:21">
-      <c r="C78" s="9" t="s">
+    <row r="124" spans="1:21">
+      <c r="C124" s="9" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="79" spans="1:21">
-      <c r="A79" s="18" t="s">
+    <row r="125" spans="1:21">
+      <c r="A125" s="18" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="80" spans="1:21" ht="201.6">
-      <c r="B80" s="9" t="s">
+    <row r="126" spans="1:21" ht="201.6">
+      <c r="B126" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="D80" s="2" t="s">
+      <c r="D126" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="82" spans="1:21">
-      <c r="A82" s="3"/>
-      <c r="B82" s="5"/>
-      <c r="C82" s="6"/>
-      <c r="D82" s="3"/>
-      <c r="F82" s="3"/>
-      <c r="G82" s="5"/>
-      <c r="H82" s="3"/>
-      <c r="I82" s="3"/>
-      <c r="K82" s="3"/>
-      <c r="L82" s="3"/>
-      <c r="M82" s="3"/>
-      <c r="N82" s="3"/>
-      <c r="P82" s="5"/>
-      <c r="Q82" s="5"/>
-      <c r="R82" s="5"/>
-      <c r="S82" s="5"/>
-      <c r="U82" s="5"/>
-    </row>
-    <row r="83" spans="1:21">
-      <c r="A83" s="1" t="s">
+    <row r="128" spans="1:21">
+      <c r="A128" s="3"/>
+      <c r="B128" s="5"/>
+      <c r="C128" s="6"/>
+      <c r="D128" s="3"/>
+      <c r="F128" s="3"/>
+      <c r="G128" s="5"/>
+      <c r="H128" s="3"/>
+      <c r="I128" s="3"/>
+      <c r="K128" s="3"/>
+      <c r="L128" s="3"/>
+      <c r="M128" s="3"/>
+      <c r="N128" s="3"/>
+      <c r="P128" s="5"/>
+      <c r="Q128" s="5"/>
+      <c r="R128" s="5"/>
+      <c r="S128" s="5"/>
+      <c r="U128" s="5"/>
+    </row>
+    <row r="129" spans="1:4">
+      <c r="A129" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C83" s="21" t="s">
+      <c r="C129" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="D83" s="2"/>
-    </row>
-    <row r="84" spans="1:21">
-      <c r="A84" s="18" t="s">
+      <c r="D129" s="2"/>
+    </row>
+    <row r="130" spans="1:4">
+      <c r="A130" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="D84" s="1" t="s">
+      <c r="D130" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="85" spans="1:21" ht="28.8">
-      <c r="C85" s="20" t="s">
+    <row r="131" spans="1:4" ht="28.8">
+      <c r="C131" s="20" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="86" spans="1:21" ht="158.4">
-      <c r="B86" s="20" t="s">
+    <row r="132" spans="1:4" ht="158.4">
+      <c r="B132" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="C86" s="20" t="s">
+      <c r="C132" s="20" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="87" spans="1:21" ht="115.2">
-      <c r="C87" s="20" t="s">
+    <row r="133" spans="1:4" ht="115.2">
+      <c r="C133" s="20" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="88" spans="1:21" ht="57.6">
-      <c r="A88" s="1" t="s">
+    <row r="134" spans="1:4" ht="57.6">
+      <c r="A134" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C88" s="20" t="s">
+      <c r="C134" s="20" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="89" spans="1:21" ht="57.6">
-      <c r="A89" s="1" t="s">
+    <row r="135" spans="1:4" ht="57.6">
+      <c r="A135" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C89" s="20" t="s">
+      <c r="C135" s="20" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="90" spans="1:21" ht="72">
-      <c r="A90" s="1" t="s">
+    <row r="136" spans="1:4" ht="72">
+      <c r="A136" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B90" s="2" t="s">
+      <c r="B136" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="C90" s="20" t="s">
+      <c r="C136" s="20" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="91" spans="1:21" ht="43.2">
-      <c r="A91" s="1" t="s">
+    <row r="137" spans="1:4" ht="43.2">
+      <c r="A137" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C91" s="20" t="s">
+      <c r="C137" s="20" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="92" spans="1:21" ht="43.2">
-      <c r="A92" s="1" t="s">
+    <row r="138" spans="1:4" ht="43.2">
+      <c r="A138" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C92" s="20" t="s">
+      <c r="C138" s="20" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="93" spans="1:21" ht="72">
-      <c r="A93" s="1" t="s">
+    <row r="139" spans="1:4" ht="72">
+      <c r="A139" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B93" s="2" t="s">
+      <c r="B139" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C93" s="20" t="s">
+      <c r="C139" s="20" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="94" spans="1:21" ht="57.6">
-      <c r="A94" s="1" t="s">
+    <row r="140" spans="1:4" ht="57.6">
+      <c r="A140" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C94" s="20" t="s">
+      <c r="C140" s="20" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="95" spans="1:21" ht="129.6">
-      <c r="A95" s="20" t="s">
+    <row r="141" spans="1:4" ht="129.6">
+      <c r="A141" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="B95" s="2" t="s">
+      <c r="B141" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="C95" s="20" t="s">
+      <c r="C141" s="20" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="96" spans="1:21" ht="100.8">
-      <c r="A96" s="20" t="s">
+    <row r="142" spans="1:4" ht="100.8">
+      <c r="A142" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="C96" s="20" t="s">
+      <c r="C142" s="20" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="97" spans="1:21" ht="144">
-      <c r="A97" s="1" t="s">
+    <row r="143" spans="1:4" ht="144">
+      <c r="A143" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C97" s="20" t="s">
+      <c r="C143" s="20" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="99" spans="1:21">
-      <c r="A99" s="3"/>
-      <c r="B99" s="5"/>
-      <c r="C99" s="6"/>
-      <c r="D99" s="3"/>
-      <c r="F99" s="3"/>
-      <c r="G99" s="5"/>
-      <c r="H99" s="3"/>
-      <c r="I99" s="3"/>
-      <c r="K99" s="3"/>
-      <c r="L99" s="3"/>
-      <c r="M99" s="3"/>
-      <c r="N99" s="3"/>
-      <c r="P99" s="5"/>
-      <c r="Q99" s="5"/>
-      <c r="R99" s="5"/>
-      <c r="S99" s="5"/>
-      <c r="U99" s="5"/>
-    </row>
-    <row r="100" spans="1:21">
-      <c r="A100" s="1" t="s">
+    <row r="145" spans="1:21">
+      <c r="A145" s="3"/>
+      <c r="B145" s="5"/>
+      <c r="C145" s="6"/>
+      <c r="D145" s="3"/>
+      <c r="F145" s="3"/>
+      <c r="G145" s="5"/>
+      <c r="H145" s="3"/>
+      <c r="I145" s="3"/>
+      <c r="K145" s="3"/>
+      <c r="L145" s="3"/>
+      <c r="M145" s="3"/>
+      <c r="N145" s="3"/>
+      <c r="P145" s="5"/>
+      <c r="Q145" s="5"/>
+      <c r="R145" s="5"/>
+      <c r="S145" s="5"/>
+      <c r="U145" s="5"/>
+    </row>
+    <row r="146" spans="1:21">
+      <c r="A146" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C100" s="22" t="s">
+      <c r="C146" s="22" t="s">
         <v>122</v>
       </c>
-      <c r="D100" s="2"/>
-    </row>
-    <row r="101" spans="1:21">
-      <c r="A101" s="18" t="s">
+      <c r="D146" s="2"/>
+    </row>
+    <row r="147" spans="1:21">
+      <c r="A147" s="18" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="102" spans="1:21">
-      <c r="A102" s="1" t="s">
+    <row r="148" spans="1:21">
+      <c r="A148" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="103" spans="1:21" ht="129.6">
-      <c r="B103" s="23" t="s">
+    <row r="149" spans="1:21" ht="129.6">
+      <c r="B149" s="23" t="s">
         <v>126</v>
       </c>
-      <c r="C103" s="23" t="s">
+      <c r="C149" s="23" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="104" spans="1:21">
-      <c r="A104" s="1" t="s">
+    <row r="150" spans="1:21">
+      <c r="A150" s="1" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="105" spans="1:21" ht="259.2">
-      <c r="B105" s="23" t="s">
+    <row r="151" spans="1:21" ht="259.2">
+      <c r="B151" s="23" t="s">
         <v>129</v>
       </c>
-      <c r="C105" s="23" t="s">
+      <c r="C151" s="23" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="106" spans="1:21" ht="28.8">
-      <c r="A106" s="23" t="s">
+    <row r="152" spans="1:21" ht="28.8">
+      <c r="A152" s="23" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="107" spans="1:21" ht="129.6">
-      <c r="B107" s="23" t="s">
+    <row r="153" spans="1:21" ht="129.6">
+      <c r="B153" s="23" t="s">
         <v>132</v>
       </c>
-      <c r="C107" s="23" t="s">
+      <c r="C153" s="23" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="108" spans="1:21">
-      <c r="A108" s="1" t="s">
+    <row r="154" spans="1:21">
+      <c r="A154" s="1" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="109" spans="1:21" ht="129.6">
-      <c r="B109" s="23" t="s">
+    <row r="155" spans="1:21" ht="129.6">
+      <c r="B155" s="23" t="s">
         <v>134</v>
       </c>
-      <c r="C109" s="23" t="s">
+      <c r="C155" s="23" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="110" spans="1:21">
-      <c r="A110" s="18" t="s">
+    <row r="156" spans="1:21">
+      <c r="A156" s="18" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="111" spans="1:21" ht="57.6">
-      <c r="B111" s="1"/>
-      <c r="C111" s="23" t="s">
+    <row r="157" spans="1:21" ht="57.6">
+      <c r="B157" s="1"/>
+      <c r="C157" s="23" t="s">
         <v>137</v>
-      </c>
-    </row>
-    <row r="112" spans="1:21" ht="28.8">
-      <c r="B112" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="C112" s="23" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" ht="43.2">
-      <c r="A113" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="B113" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="C113" s="23" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" ht="57.6">
-      <c r="A114" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B114" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="C114" s="23" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" ht="28.8">
-      <c r="A115" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="C115" s="23" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3">
-      <c r="A116" s="24" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" ht="158.4">
-      <c r="B117" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="C117" s="23" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" ht="345.6">
-      <c r="B118" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="C118" s="23" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" ht="409.6">
-      <c r="B119" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="C119" s="23" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3">
-      <c r="A120" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="C120" s="23"/>
-    </row>
-    <row r="121" spans="1:3" ht="28.8">
-      <c r="A121" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="C121" s="23" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" ht="43.2">
-      <c r="C122" s="23" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3">
-      <c r="C123" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3">
-      <c r="C124" s="23" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" ht="43.2">
-      <c r="C125" s="23" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3">
-      <c r="C126" s="23" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3">
-      <c r="A127" s="11" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" ht="57.6">
-      <c r="C128" s="23" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3">
-      <c r="C129" s="23" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3">
-      <c r="A130" s="18" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" ht="72">
-      <c r="C131" s="23" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3">
-      <c r="A132" s="11" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" ht="158.4">
-      <c r="C133" s="23" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" ht="28.8">
-      <c r="A134" s="22" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3" ht="100.8">
-      <c r="C135" s="23" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" ht="115.2">
-      <c r="B136" s="23" t="s">
-        <v>172</v>
-      </c>
-      <c r="C136" s="23" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3">
-      <c r="A137" s="11" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" ht="144">
-      <c r="B138" s="23" t="s">
-        <v>176</v>
-      </c>
-      <c r="C138" s="23" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3">
-      <c r="A139" s="11" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" ht="28.8">
-      <c r="C140" s="23" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3" ht="115.2">
-      <c r="B141" s="2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3">
-      <c r="C142" s="23" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3" ht="129.6">
-      <c r="C143" s="23" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3" ht="86.4">
-      <c r="B144" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="C144" s="23" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="146" spans="1:21">
-      <c r="A146" s="3"/>
-      <c r="B146" s="5"/>
-      <c r="C146" s="6"/>
-      <c r="D146" s="3"/>
-      <c r="F146" s="3"/>
-      <c r="G146" s="5"/>
-      <c r="H146" s="3"/>
-      <c r="I146" s="3"/>
-      <c r="K146" s="3"/>
-      <c r="L146" s="3"/>
-      <c r="M146" s="3"/>
-      <c r="N146" s="3"/>
-      <c r="P146" s="5"/>
-      <c r="Q146" s="5"/>
-      <c r="R146" s="5"/>
-      <c r="S146" s="5"/>
-      <c r="U146" s="5"/>
-    </row>
-    <row r="147" spans="1:21">
-      <c r="A147" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="C147" s="25" t="s">
-        <v>197</v>
-      </c>
-      <c r="D147" s="2"/>
-    </row>
-    <row r="148" spans="1:21">
-      <c r="A148" s="18" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="149" spans="1:21" ht="43.2">
-      <c r="C149" s="26" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="150" spans="1:21" ht="28.8">
-      <c r="A150" s="25" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="151" spans="1:21" ht="201.6">
-      <c r="A151" s="26"/>
-      <c r="B151" s="26" t="s">
-        <v>202</v>
-      </c>
-      <c r="C151" s="26" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="152" spans="1:21">
-      <c r="A152" s="11" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="153" spans="1:21" ht="57.6">
-      <c r="B153" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="C153" s="26" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="154" spans="1:21">
-      <c r="A154" s="18" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="155" spans="1:21">
-      <c r="A155" s="11" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="156" spans="1:21" ht="86.4">
-      <c r="B156" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="C156" s="26" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="157" spans="1:21">
-      <c r="A157" s="27" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="158" spans="1:21" ht="28.8">
       <c r="B158" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C158" s="23" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="159" spans="1:21" ht="43.2">
+      <c r="A159" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B159" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C159" s="23" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="160" spans="1:21" ht="57.6">
+      <c r="A160" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B160" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C160" s="23" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" ht="28.8">
+      <c r="A161" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C161" s="23" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3">
+      <c r="A162" s="24" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" ht="158.4">
+      <c r="B163" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C163" s="23" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" ht="345.6">
+      <c r="B164" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C164" s="23" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" ht="409.6">
+      <c r="B165" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C165" s="23" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3">
+      <c r="A166" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="C166" s="23"/>
+    </row>
+    <row r="167" spans="1:3" ht="28.8">
+      <c r="A167" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="C167" s="23" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" ht="43.2">
+      <c r="C168" s="23" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3">
+      <c r="C169" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3">
+      <c r="C170" s="23" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" ht="43.2">
+      <c r="C171" s="23" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3">
+      <c r="C172" s="23" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3">
+      <c r="A173" s="11" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" ht="57.6">
+      <c r="C174" s="23" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3">
+      <c r="C175" s="23" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3">
+      <c r="A176" s="18" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="177" spans="1:21" ht="72">
+      <c r="C177" s="23" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="178" spans="1:21">
+      <c r="A178" s="11" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="179" spans="1:21" ht="158.4">
+      <c r="C179" s="23" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="180" spans="1:21" ht="28.8">
+      <c r="A180" s="22" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="181" spans="1:21" ht="100.8">
+      <c r="C181" s="23" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="182" spans="1:21" ht="115.2">
+      <c r="B182" s="23" t="s">
+        <v>172</v>
+      </c>
+      <c r="C182" s="23" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="183" spans="1:21">
+      <c r="A183" s="11" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="184" spans="1:21" ht="144">
+      <c r="B184" s="23" t="s">
+        <v>176</v>
+      </c>
+      <c r="C184" s="23" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="185" spans="1:21">
+      <c r="A185" s="11" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="186" spans="1:21" ht="28.8">
+      <c r="C186" s="23" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="187" spans="1:21" ht="115.2">
+      <c r="B187" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="188" spans="1:21">
+      <c r="C188" s="23" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="189" spans="1:21" ht="129.6">
+      <c r="C189" s="23" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="190" spans="1:21" ht="86.4">
+      <c r="B190" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C190" s="23" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="192" spans="1:21">
+      <c r="A192" s="3"/>
+      <c r="B192" s="5"/>
+      <c r="C192" s="6"/>
+      <c r="D192" s="3"/>
+      <c r="F192" s="3"/>
+      <c r="G192" s="5"/>
+      <c r="H192" s="3"/>
+      <c r="I192" s="3"/>
+      <c r="K192" s="3"/>
+      <c r="L192" s="3"/>
+      <c r="M192" s="3"/>
+      <c r="N192" s="3"/>
+      <c r="P192" s="5"/>
+      <c r="Q192" s="5"/>
+      <c r="R192" s="5"/>
+      <c r="S192" s="5"/>
+      <c r="U192" s="5"/>
+    </row>
+    <row r="193" spans="1:4">
+      <c r="A193" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C193" s="25" t="s">
+        <v>197</v>
+      </c>
+      <c r="D193" s="2"/>
+    </row>
+    <row r="194" spans="1:4">
+      <c r="A194" s="18" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" ht="43.2">
+      <c r="C195" s="26" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" ht="28.8">
+      <c r="A196" s="25" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" ht="201.6">
+      <c r="A197" s="26"/>
+      <c r="B197" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="C197" s="26" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4">
+      <c r="A198" s="11" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" ht="57.6">
+      <c r="B199" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C199" s="26" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4">
+      <c r="A200" s="18" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4">
+      <c r="A201" s="11" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" ht="86.4">
+      <c r="B202" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="C202" s="26" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4">
+      <c r="A203" s="27" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" ht="28.8">
+      <c r="B204" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="C158" s="26" t="s">
+      <c r="C204" s="26" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="159" spans="1:21">
-      <c r="A159" s="11" t="s">
+    <row r="205" spans="1:4">
+      <c r="A205" s="11" t="s">
         <v>211</v>
       </c>
-      <c r="C159" s="29" t="s">
+      <c r="C205" s="29" t="s">
         <v>233</v>
       </c>
-      <c r="D159" s="28" t="s">
+      <c r="D205" s="28" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="160" spans="1:21" ht="57.6">
-      <c r="C160" s="26" t="s">
+    <row r="206" spans="1:4" ht="57.6">
+      <c r="C206" s="26" t="s">
         <v>242</v>
       </c>
-      <c r="D160" s="26" t="s">
+      <c r="D206" s="26" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="161" spans="1:4" ht="28.8">
-      <c r="C161" s="26" t="s">
+    <row r="207" spans="1:4" ht="28.8">
+      <c r="C207" s="26" t="s">
         <v>243</v>
       </c>
-      <c r="D161" s="26" t="s">
+      <c r="D207" s="26" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="162" spans="1:4">
-      <c r="A162" s="11" t="s">
+    <row r="208" spans="1:4">
+      <c r="A208" s="11" t="s">
         <v>212</v>
       </c>
-      <c r="C162" s="29" t="s">
+      <c r="C208" s="29" t="s">
         <v>233</v>
       </c>
-      <c r="D162" s="28" t="s">
+      <c r="D208" s="28" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="163" spans="1:4" ht="57.6">
-      <c r="B163" s="2" t="s">
+    <row r="209" spans="1:4" ht="57.6">
+      <c r="B209" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="C163" s="2" t="s">
+      <c r="C209" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="D163" s="26" t="s">
+      <c r="D209" s="26" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="164" spans="1:4">
-      <c r="A164" s="19" t="s">
+    <row r="210" spans="1:4">
+      <c r="A210" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="C164" s="29" t="s">
+      <c r="C210" s="29" t="s">
         <v>233</v>
       </c>
-      <c r="D164" s="28" t="s">
+      <c r="D210" s="28" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="165" spans="1:4" ht="115.2">
-      <c r="C165" s="2" t="s">
+    <row r="211" spans="1:4" ht="115.2">
+      <c r="C211" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="D165" s="2" t="s">
+      <c r="D211" s="2" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="166" spans="1:4" ht="86.4">
-      <c r="C166" s="2" t="s">
+    <row r="212" spans="1:4" ht="86.4">
+      <c r="C212" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="D166" s="26" t="s">
+      <c r="D212" s="26" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="167" spans="1:4">
-      <c r="A167" s="19" t="s">
+    <row r="213" spans="1:4">
+      <c r="A213" s="19" t="s">
         <v>218</v>
       </c>
-      <c r="C167" s="29" t="s">
+      <c r="C213" s="29" t="s">
         <v>233</v>
       </c>
-      <c r="D167" s="28" t="s">
+      <c r="D213" s="28" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="168" spans="1:4" ht="57.6">
-      <c r="A168" s="2" t="s">
+    <row r="214" spans="1:4" ht="57.6">
+      <c r="A214" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="C168" s="26" t="s">
+      <c r="C214" s="26" t="s">
         <v>221</v>
       </c>
-      <c r="D168" s="26" t="s">
+      <c r="D214" s="26" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="169" spans="1:4" ht="100.8">
-      <c r="A169" s="2" t="s">
+    <row r="215" spans="1:4" ht="100.8">
+      <c r="A215" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="C169" s="26" t="s">
+      <c r="C215" s="26" t="s">
         <v>238</v>
       </c>
-      <c r="D169" s="2" t="s">
+      <c r="D215" s="2" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="170" spans="1:4" ht="201.6">
-      <c r="A170" s="2" t="s">
+    <row r="216" spans="1:4" ht="201.6">
+      <c r="A216" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="C170" s="26" t="s">
+      <c r="C216" s="26" t="s">
         <v>240</v>
       </c>
-      <c r="D170" s="2" t="s">
+      <c r="D216" s="2" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="171" spans="1:4">
-      <c r="A171" s="19" t="s">
+    <row r="217" spans="1:4">
+      <c r="A217" s="19" t="s">
         <v>209</v>
       </c>
-      <c r="C171" s="29" t="s">
+      <c r="C217" s="29" t="s">
         <v>233</v>
       </c>
-      <c r="D171" s="28" t="s">
+      <c r="D217" s="28" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="172" spans="1:4" ht="158.4">
-      <c r="C172" s="26" t="s">
+    <row r="218" spans="1:4" ht="158.4">
+      <c r="C218" s="26" t="s">
         <v>224</v>
       </c>
-      <c r="D172" s="26" t="s">
+      <c r="D218" s="26" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="173" spans="1:4">
-      <c r="A173" s="19" t="s">
+    <row r="219" spans="1:4">
+      <c r="A219" s="19" t="s">
         <v>228</v>
       </c>
-      <c r="C173" s="29" t="s">
+      <c r="C219" s="29" t="s">
         <v>233</v>
       </c>
-      <c r="D173" s="28" t="s">
+      <c r="D219" s="28" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="174" spans="1:4" ht="57.6">
-      <c r="A174" s="2" t="s">
+    <row r="220" spans="1:4" ht="57.6">
+      <c r="A220" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="C174" s="26" t="s">
+      <c r="C220" s="26" t="s">
         <v>230</v>
       </c>
-      <c r="D174" s="2" t="s">
+      <c r="D220" s="2" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="175" spans="1:4" ht="129.6">
-      <c r="A175" s="2" t="s">
+    <row r="221" spans="1:4" ht="129.6">
+      <c r="A221" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="C175" s="2" t="s">
+      <c r="C221" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="D175" s="26" t="s">
+      <c r="D221" s="26" t="s">
         <v>234</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1" xr:uid="{E59BE88A-E81B-4A5C-9ABF-D0B1D72A17A8}"/>
   </hyperlinks>

</xml_diff>